<commit_message>
Added function to see if there was no output file selected
Made the program able to parse empty files

Added empty file test to test_merge.py

Fixed the recursive function
</commit_message>
<xml_diff>
--- a/src/confluence/test_files/newfile.xlsx
+++ b/src/confluence/test_files/newfile.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -377,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -397,21 +398,49 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>5</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>6</v>
       </c>
-      <c r="B3">
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
         <v>3</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>